<commit_message>
release version 1.0.0 update all sensor can use.
</commit_message>
<xml_diff>
--- a/full_waterproof_temperature_sensor/full_waterproof_temperature_sensor_calibration.xlsx
+++ b/full_waterproof_temperature_sensor/full_waterproof_temperature_sensor_calibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\Coding\Arduino\cyber_physical_system_and_sensor\full_waterproof_temperature_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8641D1CA-277F-4B59-BAD0-E759C746F626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA829A2F-ECE8-46AD-911A-7F5F66C56DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9E1DC5AF-41CF-462C-962B-EC8496DA7A7E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E1DC5AF-41CF-462C-962B-EC8496DA7A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Calibration" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <r>
+      <t xml:space="preserve">Calibrated Sensor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Full Water proof Temperature Sensor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This Excel sheet is for calibrated in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Linear Calibration </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with Full Waterproof Temperature Sensor</t>
+    </r>
+  </si>
+  <si>
+    <t>Sensor [C]</t>
+  </si>
+  <si>
+    <t>จุดเดือด [C]</t>
+  </si>
+  <si>
+    <t>จุดเยือกแข็ง [C]</t>
+  </si>
+  <si>
+    <t>After Sensor [C]</t>
+  </si>
+  <si>
+    <t>ERROR [%]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,13 +109,92 @@
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,14 +209,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,6 +242,1183 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="th-TH"/>
+              <a:t>กราฟความสัมพันธ์ระหว่างอุณหภูมิที่ยังไม่ปรับเทียบ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="th-TH" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="th-TH" baseline="0"/>
+              <a:t>กับมีการปรับเทียบ </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>[C]</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Linear Calibration'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>After Sensor [C]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10543196280067706"/>
+                  <c:y val="1.0727278276261978E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Linear Calibration'!$A$5:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.87</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Linear Calibration'!$B$5:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-0.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ABA6-4CB7-A5BD-F54AF881A2AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608559024"/>
+        <c:axId val="522972864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608559024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature Sensor (Calibrated)[C]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522972864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="522972864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Sensor (Uncalibrated)[C]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608559024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10180</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>207064</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0928218-D7AA-0308-1256-2D21679F9486}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,15 +1738,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B059518-0250-4168-9EE0-582A42935380}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.31</v>
+      </c>
+      <c r="B5">
+        <v>-0.06</v>
+      </c>
+      <c r="C5">
+        <f>ROUND(ABS(((B5-A5)/B5)*100),2)</f>
+        <v>616.66999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B7">
+        <v>0.19</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C14" si="0">ROUND(ABS(((B7-A7)/B7)*100),2)</f>
+        <v>194.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.81</v>
+      </c>
+      <c r="B8">
+        <v>0.44</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>84.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1.19</v>
+      </c>
+      <c r="B9">
+        <v>0.82</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>45.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>14.81</v>
+      </c>
+      <c r="B10">
+        <v>14.44</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>14.63</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="B12">
+        <v>15.82</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>20.69</v>
+      </c>
+      <c r="B13">
+        <v>20.32</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>21.87</v>
+      </c>
+      <c r="B14">
+        <v>21.5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>91.62</v>
+      </c>
+      <c r="B15">
+        <v>91.25</v>
+      </c>
+      <c r="C15">
+        <f>ROUND(ABS(((B15-A15)/B15)*100),2)</f>
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>91.56</v>
+      </c>
+      <c r="B16" s="3">
+        <v>91.12</v>
+      </c>
+      <c r="C16">
+        <f>ROUND(ABS(((B16-A16)/B16)*100),2)</f>
+        <v>0.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -420,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423A82D9-483F-4DCB-A83B-647F44321C3A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>